<commit_message>
update raw data with pivot tables
</commit_message>
<xml_diff>
--- a/raw_data/baltimore_city_minimum_wage_FRED.xlsx
+++ b/raw_data/baltimore_city_minimum_wage_FRED.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melanieshimano/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melanieshimano/Desktop/multiple_regression_analysis/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C231C5D7-E741-974F-838C-552A8F83F39F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B3D8B072-50B3-D34A-B49E-536DB7B44825}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="1960" windowWidth="26840" windowHeight="15540"/>
+    <workbookView xWindow="1580" yWindow="1960" windowWidth="26840" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="baltimore_city_minimum_wage_FRE" sheetId="1" r:id="rId1"/>
@@ -36,8 +36,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -514,9 +514,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -871,22 +872,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="d">
         <v>1968-01-01</v>
       </c>
@@ -894,7 +898,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="d">
         <v>1969-01-01</v>
       </c>
@@ -902,7 +906,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="d">
         <v>1970-01-01</v>
       </c>
@@ -910,7 +914,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="d">
         <v>1971-01-01</v>
       </c>
@@ -918,7 +922,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="d">
         <v>1972-01-01</v>
       </c>
@@ -926,7 +930,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="d">
         <v>1973-01-01</v>
       </c>
@@ -934,7 +938,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="d">
         <v>1974-01-01</v>
       </c>
@@ -942,7 +946,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="d">
         <v>1975-01-01</v>
       </c>
@@ -950,7 +954,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="d">
         <v>1976-01-01</v>
       </c>
@@ -958,7 +962,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="d">
         <v>1977-01-01</v>
       </c>
@@ -966,7 +970,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" s="1" t="d">
         <v>1978-01-01</v>
       </c>
@@ -974,7 +978,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" s="1" t="d">
         <v>1979-01-01</v>
       </c>
@@ -982,7 +986,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" s="1" t="d">
         <v>1980-01-01</v>
       </c>
@@ -990,7 +994,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" s="1" t="d">
         <v>1981-01-01</v>
       </c>
@@ -998,7 +1002,7 @@
         <v>3.35</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16" s="1" t="d">
         <v>1982-01-01</v>
       </c>
@@ -1006,7 +1010,7 @@
         <v>3.35</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" s="1" t="d">
         <v>1983-01-01</v>
       </c>
@@ -1014,7 +1018,7 @@
         <v>3.35</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" s="1" t="d">
         <v>1984-01-01</v>
       </c>
@@ -1022,7 +1026,7 @@
         <v>3.35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" s="1" t="d">
         <v>1985-01-01</v>
       </c>
@@ -1030,7 +1034,7 @@
         <v>3.35</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" s="1" t="d">
         <v>1986-01-01</v>
       </c>
@@ -1038,7 +1042,7 @@
         <v>3.35</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" s="1" t="d">
         <v>1987-01-01</v>
       </c>
@@ -1046,7 +1050,7 @@
         <v>3.35</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" s="1" t="d">
         <v>1988-01-01</v>
       </c>
@@ -1054,7 +1058,7 @@
         <v>3.35</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23" s="1" t="d">
         <v>1989-01-01</v>
       </c>
@@ -1062,7 +1066,7 @@
         <v>3.35</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24" s="1" t="d">
         <v>1990-01-01</v>
       </c>
@@ -1070,7 +1074,7 @@
         <v>3.35</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2">
       <c r="A25" s="1" t="d">
         <v>1991-01-01</v>
       </c>
@@ -1078,7 +1082,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="A26" s="1" t="d">
         <v>1992-01-01</v>
       </c>
@@ -1086,7 +1090,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2">
       <c r="A27" s="1" t="d">
         <v>1993-01-01</v>
       </c>
@@ -1094,7 +1098,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2">
       <c r="A28" s="1" t="d">
         <v>1994-01-01</v>
       </c>
@@ -1102,7 +1106,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2">
       <c r="A29" s="1" t="d">
         <v>1995-01-01</v>
       </c>
@@ -1110,7 +1114,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2">
       <c r="A30" s="1" t="d">
         <v>1996-01-01</v>
       </c>
@@ -1118,7 +1122,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2">
       <c r="A31" s="1" t="d">
         <v>1997-01-01</v>
       </c>
@@ -1126,7 +1130,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2">
       <c r="A32" s="1" t="d">
         <v>1998-01-01</v>
       </c>
@@ -1134,7 +1138,7 @@
         <v>5.15</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2">
       <c r="A33" s="1" t="d">
         <v>1999-01-01</v>
       </c>
@@ -1142,7 +1146,7 @@
         <v>5.15</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2">
       <c r="A34" s="1" t="d">
         <v>2000-01-01</v>
       </c>
@@ -1150,7 +1154,7 @@
         <v>5.15</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2">
       <c r="A35" s="1" t="d">
         <v>2001-01-01</v>
       </c>
@@ -1158,7 +1162,7 @@
         <v>5.15</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2">
       <c r="A36" s="1" t="d">
         <v>2002-01-01</v>
       </c>
@@ -1166,7 +1170,7 @@
         <v>5.15</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2">
       <c r="A37" s="1" t="d">
         <v>2003-01-01</v>
       </c>
@@ -1174,7 +1178,7 @@
         <v>5.15</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2">
       <c r="A38" s="1" t="d">
         <v>2004-01-01</v>
       </c>
@@ -1182,7 +1186,7 @@
         <v>5.15</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2">
       <c r="A39" s="1" t="d">
         <v>2005-01-01</v>
       </c>
@@ -1190,7 +1194,7 @@
         <v>5.15</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2">
       <c r="A40" s="1" t="d">
         <v>2006-01-01</v>
       </c>
@@ -1198,7 +1202,7 @@
         <v>5.15</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2">
       <c r="A41" s="1" t="d">
         <v>2007-01-01</v>
       </c>
@@ -1206,7 +1210,7 @@
         <v>6.15</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2">
       <c r="A42" s="1" t="d">
         <v>2008-01-01</v>
       </c>
@@ -1214,7 +1218,7 @@
         <v>6.15</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2">
       <c r="A43" s="1" t="d">
         <v>2009-01-01</v>
       </c>
@@ -1222,7 +1226,7 @@
         <v>6.55</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2">
       <c r="A44" s="1" t="d">
         <v>2010-01-01</v>
       </c>
@@ -1230,7 +1234,7 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2">
       <c r="A45" s="1" t="d">
         <v>2011-01-01</v>
       </c>
@@ -1238,7 +1242,7 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2">
       <c r="A46" s="1" t="d">
         <v>2012-01-01</v>
       </c>
@@ -1246,7 +1250,7 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2">
       <c r="A47" s="1" t="d">
         <v>2013-01-01</v>
       </c>
@@ -1254,7 +1258,7 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2">
       <c r="A48" s="1" t="d">
         <v>2014-01-01</v>
       </c>
@@ -1262,7 +1266,7 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2">
       <c r="A49" s="1" t="d">
         <v>2015-01-01</v>
       </c>
@@ -1270,7 +1274,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2">
       <c r="A50" s="1" t="d">
         <v>2016-01-01</v>
       </c>
@@ -1278,7 +1282,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2">
       <c r="A51" s="1" t="d">
         <v>2017-01-01</v>
       </c>
@@ -1286,7 +1290,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2">
       <c r="A52" s="1" t="d">
         <v>2018-01-01</v>
       </c>
@@ -1294,7 +1298,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2">
       <c r="A53" s="1" t="d">
         <v>2019-01-01</v>
       </c>

</xml_diff>